<commit_message>
Working on Sum of random variables exercises
</commit_message>
<xml_diff>
--- a/Homework/JulySumofMVSDHW.xlsx
+++ b/Homework/JulySumofMVSDHW.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\edxtake2module1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\Stats using Excel\stats-primer\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD19ED83-5CEA-480E-BB4D-DAF7D7BEFC26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Homework 3_3</t>
   </si>
@@ -72,12 +78,21 @@
   </si>
   <si>
     <t>variance and standard deviation of your winnings.</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,26 +425,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -437,8 +457,23 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <f>1/36</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="K3">
+        <f>I3*J3</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="M3">
+        <f>((I3-$K$14)^2)*J3</f>
+        <v>0.6944444444444442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -447,8 +482,23 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4">
+        <f>2/36</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K13" si="0">I4*J4</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M13" si="1">((I4-$K$14)^2)*J4</f>
+        <v>0.8888888888888884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -457,8 +507,40 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="4">
+        <f>3/36</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>0.74999999999999956</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4">
+        <f>4/36</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -467,8 +549,23 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" s="4">
+        <f>5/36</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.13888888888888865</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -477,8 +574,23 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" s="4">
+        <f>6/36</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>1.3147681753683529E-31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -487,8 +599,22 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>0.13888888888888914</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -497,8 +623,23 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" s="4">
+        <f>4/36</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -507,8 +648,23 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
+        <f>3/36</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000044</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -517,8 +673,23 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12" s="4">
+        <f>2/36</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>0.88888888888888928</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -527,8 +698,23 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <f>1/36</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M13">
+        <f>((I13-$K$14)^2)*J13</f>
+        <v>0.69444444444444464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -537,8 +723,26 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="4">
+        <f>SUM(K3:K13)</f>
+        <v>6.9999999999999991</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="4">
+        <f>SUM(M3:M13)</f>
+        <v>5.8333333333333339</v>
+      </c>
+      <c r="N14">
+        <f>M14*50</f>
+        <v>291.66666666666669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -548,8 +752,19 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15">
+        <f>M14^(1/2)</f>
+        <v>2.4152294576982398</v>
+      </c>
+      <c r="N15">
+        <f>N14^(1/2)</f>
+        <v>17.078251276599332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -560,7 +775,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -571,6 +786,68 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>35</v>
+      </c>
+      <c r="F20">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="G20">
+        <f>E20*F20</f>
+        <v>0.92105263157894735</v>
+      </c>
+      <c r="I20">
+        <f>((E20-G22)^2)*F20</f>
+        <v>32.333867910774167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>-1</v>
+      </c>
+      <c r="F21">
+        <f>37/38</f>
+        <v>0.97368421052631582</v>
+      </c>
+      <c r="G21">
+        <f>E21*F21</f>
+        <v>-0.97368421052631582</v>
+      </c>
+      <c r="I21">
+        <f>((E21-G22)^2)*F21</f>
+        <v>0.87388832191281518</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f>SUM(G20:G21)</f>
+        <v>-5.2631578947368474E-2</v>
+      </c>
+      <c r="I22">
+        <f>SUM(I20:I21)</f>
+        <v>33.207756232686982</v>
+      </c>
+      <c r="J22">
+        <f>I22*100</f>
+        <v>3320.7756232686984</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f>G22*100</f>
+        <v>-5.2631578947368478</v>
+      </c>
+      <c r="I23">
+        <f>I22^(1/2)</f>
+        <v>5.7626171339667343</v>
+      </c>
+      <c r="J23">
+        <f>J22^(1/2)</f>
+        <v>57.626171339667344</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>